<commit_message>
"datetime" split into "date" and "time"
</commit_message>
<xml_diff>
--- a/Working Minutes.xlsx
+++ b/Working Minutes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5c5378f3fcb43b9/Dokumente/Berufseinstieg/Sprachtechnologie/Predicting_Bike_Rental_Demand/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="11_92483E2D04E89AD36523F29B863E8C1851038389" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9FCD4BB-6321-4A68-97F3-15A3F15B2C30}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="11_92483E2D04E89AD36523F29B863E8C1851038389" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABECF7C1-D12D-428D-96E6-F203161FBACB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,7 +453,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="DG2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DK10" sqref="DK10"/>
+      <selection pane="bottomRight" activeCell="DU8" sqref="DU8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="D7" s="7">
         <f t="shared" ref="D7" si="0">SUM(E7:AAA7)</f>
-        <v>845</v>
+        <v>870</v>
       </c>
       <c r="E7">
         <v>60</v>
@@ -1195,6 +1195,9 @@
       <c r="DN7">
         <f>25+25+25+15</f>
         <v>90</v>
+      </c>
+      <c r="DU7">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Training and validation sets completed, except for dependent variable in validation set
</commit_message>
<xml_diff>
--- a/Working Minutes.xlsx
+++ b/Working Minutes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5c5378f3fcb43b9/Dokumente/Berufseinstieg/Sprachtechnologie/Predicting_Bike_Rental_Demand/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="11_92483E2D04E89AD36523F29B863E8C1851038389" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE85FD2B-BEF0-455D-A0B0-DA0667540995}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{03873DD5-F6D7-47D6-91AE-953341A440FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE0BFD43-1962-4CEC-BA6D-BE4A07F210DA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -450,10 +450,10 @@
   <dimension ref="A1:GP7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="DM2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="DQ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="EA8" sqref="EA8"/>
+      <selection pane="bottomRight" activeCell="ED8" sqref="ED8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="D7" s="7">
         <f t="shared" ref="D7" si="0">SUM(E7:AAA7)</f>
-        <v>895</v>
+        <v>950</v>
       </c>
       <c r="E7">
         <v>60</v>
@@ -1201,6 +1201,12 @@
       </c>
       <c r="EA7">
         <v>25</v>
+      </c>
+      <c r="EB7">
+        <v>25</v>
+      </c>
+      <c r="ED7">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Training and validation sets completed
</commit_message>
<xml_diff>
--- a/Working Minutes.xlsx
+++ b/Working Minutes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5c5378f3fcb43b9/Dokumente/Berufseinstieg/Sprachtechnologie/Predicting_Bike_Rental_Demand/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{03873DD5-F6D7-47D6-91AE-953341A440FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE0BFD43-1962-4CEC-BA6D-BE4A07F210DA}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{03873DD5-F6D7-47D6-91AE-953341A440FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E4E5D84-3A24-44D4-B18C-BC8AA6C91A41}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Task</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Build package "CsvDataset"</t>
+  </si>
+  <si>
+    <t>Research: How to do a unit test</t>
   </si>
 </sst>
 </file>
@@ -447,13 +450,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:GP7"/>
+  <dimension ref="A1:GP8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="DQ2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="EL2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="ED8" sqref="ED8"/>
+      <selection pane="bottomRight" activeCell="EV6" sqref="EV6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1137,9 +1140,12 @@
       <c r="B7" s="7">
         <v>18</v>
       </c>
+      <c r="C7" s="8">
+        <v>44519</v>
+      </c>
       <c r="D7" s="7">
-        <f t="shared" ref="D7" si="0">SUM(E7:AAA7)</f>
-        <v>950</v>
+        <f t="shared" ref="D7:D8" si="0">SUM(E7:AAA7)</f>
+        <v>1140</v>
       </c>
       <c r="E7">
         <v>60</v>
@@ -1207,6 +1213,30 @@
       </c>
       <c r="ED7">
         <v>30</v>
+      </c>
+      <c r="EI7">
+        <v>150</v>
+      </c>
+      <c r="EJ7">
+        <v>25</v>
+      </c>
+      <c r="EL7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:198" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="7">
+        <v>19</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="EL8">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set up Training file, added validation set as csv
</commit_message>
<xml_diff>
--- a/Working Minutes.xlsx
+++ b/Working Minutes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5c5378f3fcb43b9/Dokumente/Berufseinstieg/Sprachtechnologie/Predicting_Bike_Rental_Demand/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{03873DD5-F6D7-47D6-91AE-953341A440FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E4E5D84-3A24-44D4-B18C-BC8AA6C91A41}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{03873DD5-F6D7-47D6-91AE-953341A440FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F42690CF-35E7-43D7-A84C-EB0FD218D13E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Task</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Research: How to do a unit test</t>
+  </si>
+  <si>
+    <t>Re-install scikit-learn</t>
+  </si>
+  <si>
+    <t>Train Set</t>
   </si>
 </sst>
 </file>
@@ -450,13 +456,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:GP8"/>
+  <dimension ref="A1:GP10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="EL2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="FF2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="EV6" sqref="EV6"/>
+      <selection pane="bottomRight" activeCell="FR11" sqref="FR11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1144,7 +1150,7 @@
         <v>44519</v>
       </c>
       <c r="D7" s="7">
-        <f t="shared" ref="D7:D8" si="0">SUM(E7:AAA7)</f>
+        <f t="shared" ref="D7:D10" si="0">SUM(E7:AAA7)</f>
         <v>1140</v>
       </c>
       <c r="E7">
@@ -1233,10 +1239,46 @@
       </c>
       <c r="D8" s="7">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="EL8">
         <v>10</v>
+      </c>
+      <c r="FC8">
+        <v>50</v>
+      </c>
+      <c r="FD8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:198" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="FL9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:198" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="7">
+        <v>23</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="FQ10">
+        <v>25</v>
+      </c>
+      <c r="FR10">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>